<commit_message>
Demultiplexing report almost done
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/micans_v6_exp1_plexed/metadata_plexed.xlsx
+++ b/metadata/excel/projects/micans_v6_exp1_plexed/metadata_plexed.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="312">
   <si>
     <t>Country</t>
   </si>
@@ -1051,6 +1051,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Multiplexed samples recieved from BaseSpace by Micans on 15th of May 2016 (Experiment 1)</t>
   </si>
 </sst>
 </file>
@@ -2380,10 +2383,10 @@
   </sheetPr>
   <dimension ref="A1:CD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="X32" sqref="X32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2772,7 +2775,7 @@
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
-        <f>COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BQ3,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" ref="A3:A38" si="0">COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BQ3,"&lt;&gt;"&amp;"")</f>
         <v>1</v>
       </c>
       <c r="B3" s="27">
@@ -2829,7 +2832,12 @@
       <c r="W3" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="1"/>
+      <c r="Y3" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA3" s="49" t="s">
         <v>152</v>
       </c>
@@ -2919,7 +2927,7 @@
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
-        <f>COUNTIF(D4,"&lt;&gt;"&amp;"")+COUNTIF(BQ4,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B4" s="27">
@@ -2976,7 +2984,12 @@
       <c r="W4" t="s">
         <v>49</v>
       </c>
-      <c r="Z4" s="1"/>
+      <c r="Y4" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA4" s="49" t="s">
         <v>152</v>
       </c>
@@ -3066,7 +3079,7 @@
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
-        <f>COUNTIF(D5,"&lt;&gt;"&amp;"")+COUNTIF(BQ5,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B5" s="27">
@@ -3123,7 +3136,12 @@
       <c r="W5" t="s">
         <v>49</v>
       </c>
-      <c r="Z5" s="1"/>
+      <c r="Y5" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA5" s="49" t="s">
         <v>152</v>
       </c>
@@ -3213,7 +3231,7 @@
     </row>
     <row r="6" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
-        <f>COUNTIF(D6,"&lt;&gt;"&amp;"")+COUNTIF(BQ6,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B6" s="27">
@@ -3270,7 +3288,12 @@
       <c r="W6" t="s">
         <v>49</v>
       </c>
-      <c r="Z6" s="1"/>
+      <c r="Y6" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA6" s="49" t="s">
         <v>152</v>
       </c>
@@ -3360,7 +3383,7 @@
     </row>
     <row r="7" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
-        <f>COUNTIF(D7,"&lt;&gt;"&amp;"")+COUNTIF(BQ7,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B7" s="27">
@@ -3417,7 +3440,12 @@
       <c r="W7" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" s="1"/>
+      <c r="Y7" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA7" s="49" t="s">
         <v>152</v>
       </c>
@@ -3507,7 +3535,7 @@
     </row>
     <row r="8" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
-        <f>COUNTIF(D8,"&lt;&gt;"&amp;"")+COUNTIF(BQ8,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8" s="27">
@@ -3564,7 +3592,12 @@
       <c r="W8" t="s">
         <v>49</v>
       </c>
-      <c r="Z8" s="1"/>
+      <c r="Y8" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA8" s="49" t="s">
         <v>152</v>
       </c>
@@ -3654,7 +3687,7 @@
     </row>
     <row r="9" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
-        <f>COUNTIF(D9,"&lt;&gt;"&amp;"")+COUNTIF(BQ9,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B9" s="27">
@@ -3711,7 +3744,12 @@
       <c r="W9" t="s">
         <v>49</v>
       </c>
-      <c r="Z9" s="1"/>
+      <c r="Y9" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA9" s="49" t="s">
         <v>152</v>
       </c>
@@ -3801,7 +3839,7 @@
     </row>
     <row r="10" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
-        <f>COUNTIF(D10,"&lt;&gt;"&amp;"")+COUNTIF(BQ10,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B10" s="27">
@@ -3858,7 +3896,12 @@
       <c r="W10" t="s">
         <v>49</v>
       </c>
-      <c r="Z10" s="1"/>
+      <c r="Y10" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA10" s="49" t="s">
         <v>152</v>
       </c>
@@ -3948,7 +3991,7 @@
     </row>
     <row r="11" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
-        <f>COUNTIF(D11,"&lt;&gt;"&amp;"")+COUNTIF(BQ11,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B11" s="27">
@@ -4005,7 +4048,12 @@
       <c r="W11" t="s">
         <v>49</v>
       </c>
-      <c r="Z11" s="1"/>
+      <c r="Y11" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA11" s="49" t="s">
         <v>152</v>
       </c>
@@ -4095,7 +4143,7 @@
     </row>
     <row r="12" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
-        <f>COUNTIF(D12,"&lt;&gt;"&amp;"")+COUNTIF(BQ12,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B12" s="27">
@@ -4152,7 +4200,12 @@
       <c r="W12" t="s">
         <v>49</v>
       </c>
-      <c r="Z12" s="1"/>
+      <c r="Y12" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA12" s="49" t="s">
         <v>152</v>
       </c>
@@ -4242,7 +4295,7 @@
     </row>
     <row r="13" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
-        <f>COUNTIF(D13,"&lt;&gt;"&amp;"")+COUNTIF(BQ13,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B13" s="27">
@@ -4299,7 +4352,12 @@
       <c r="W13" t="s">
         <v>49</v>
       </c>
-      <c r="Z13" s="1"/>
+      <c r="Y13" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA13" s="49" t="s">
         <v>152</v>
       </c>
@@ -4389,7 +4447,7 @@
     </row>
     <row r="14" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
-        <f>COUNTIF(D14,"&lt;&gt;"&amp;"")+COUNTIF(BQ14,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B14" s="27">
@@ -4446,7 +4504,12 @@
       <c r="W14" t="s">
         <v>49</v>
       </c>
-      <c r="Z14" s="1"/>
+      <c r="Y14" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA14" s="49" t="s">
         <v>152</v>
       </c>
@@ -4536,7 +4599,7 @@
     </row>
     <row r="15" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
-        <f>COUNTIF(D15,"&lt;&gt;"&amp;"")+COUNTIF(BQ15,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B15" s="27">
@@ -4593,7 +4656,12 @@
       <c r="W15" t="s">
         <v>49</v>
       </c>
-      <c r="Z15" s="1"/>
+      <c r="Y15" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA15" s="49" t="s">
         <v>152</v>
       </c>
@@ -4683,7 +4751,7 @@
     </row>
     <row r="16" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
-        <f>COUNTIF(D16,"&lt;&gt;"&amp;"")+COUNTIF(BQ16,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B16" s="27">
@@ -4740,7 +4808,12 @@
       <c r="W16" t="s">
         <v>49</v>
       </c>
-      <c r="Z16" s="1"/>
+      <c r="Y16" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA16" s="49" t="s">
         <v>152</v>
       </c>
@@ -4830,7 +4903,7 @@
     </row>
     <row r="17" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
-        <f>COUNTIF(D17,"&lt;&gt;"&amp;"")+COUNTIF(BQ17,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B17" s="27">
@@ -4887,7 +4960,12 @@
       <c r="W17" t="s">
         <v>49</v>
       </c>
-      <c r="Z17" s="1"/>
+      <c r="Y17" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA17" s="49" t="s">
         <v>152</v>
       </c>
@@ -4977,7 +5055,7 @@
     </row>
     <row r="18" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
-        <f>COUNTIF(D18,"&lt;&gt;"&amp;"")+COUNTIF(BQ18,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B18" s="27">
@@ -5034,7 +5112,12 @@
       <c r="W18" t="s">
         <v>49</v>
       </c>
-      <c r="Z18" s="1"/>
+      <c r="Y18" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA18" s="49" t="s">
         <v>152</v>
       </c>
@@ -5124,7 +5207,7 @@
     </row>
     <row r="19" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
-        <f>COUNTIF(D19,"&lt;&gt;"&amp;"")+COUNTIF(BQ19,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B19" s="27">
@@ -5181,7 +5264,12 @@
       <c r="W19" t="s">
         <v>49</v>
       </c>
-      <c r="Z19" s="1"/>
+      <c r="Y19" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA19" s="49" t="s">
         <v>152</v>
       </c>
@@ -5271,7 +5359,7 @@
     </row>
     <row r="20" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
-        <f>COUNTIF(D20,"&lt;&gt;"&amp;"")+COUNTIF(BQ20,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B20" s="27">
@@ -5328,7 +5416,12 @@
       <c r="W20" t="s">
         <v>49</v>
       </c>
-      <c r="Z20" s="1"/>
+      <c r="Y20" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA20" s="49" t="s">
         <v>152</v>
       </c>
@@ -5418,7 +5511,7 @@
     </row>
     <row r="21" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
-        <f>COUNTIF(D21,"&lt;&gt;"&amp;"")+COUNTIF(BQ21,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B21" s="27">
@@ -5475,7 +5568,12 @@
       <c r="W21" t="s">
         <v>49</v>
       </c>
-      <c r="Z21" s="1"/>
+      <c r="Y21" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA21" s="49" t="s">
         <v>152</v>
       </c>
@@ -5565,7 +5663,7 @@
     </row>
     <row r="22" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
-        <f>COUNTIF(D22,"&lt;&gt;"&amp;"")+COUNTIF(BQ22,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B22" s="27">
@@ -5622,7 +5720,12 @@
       <c r="W22" t="s">
         <v>49</v>
       </c>
-      <c r="Z22" s="1"/>
+      <c r="Y22" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA22" s="49" t="s">
         <v>152</v>
       </c>
@@ -5712,7 +5815,7 @@
     </row>
     <row r="23" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
-        <f>COUNTIF(D23,"&lt;&gt;"&amp;"")+COUNTIF(BQ23,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B23" s="27">
@@ -5769,7 +5872,12 @@
       <c r="W23" t="s">
         <v>49</v>
       </c>
-      <c r="Z23" s="1"/>
+      <c r="Y23" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA23" s="49" t="s">
         <v>152</v>
       </c>
@@ -5859,7 +5967,7 @@
     </row>
     <row r="24" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
-        <f>COUNTIF(D24,"&lt;&gt;"&amp;"")+COUNTIF(BQ24,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B24" s="27">
@@ -5916,7 +6024,12 @@
       <c r="W24" t="s">
         <v>49</v>
       </c>
-      <c r="Z24" s="1"/>
+      <c r="Y24" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA24" s="49" t="s">
         <v>152</v>
       </c>
@@ -6006,7 +6119,7 @@
     </row>
     <row r="25" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
-        <f>COUNTIF(D25,"&lt;&gt;"&amp;"")+COUNTIF(BQ25,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B25" s="27">
@@ -6063,7 +6176,12 @@
       <c r="W25" t="s">
         <v>49</v>
       </c>
-      <c r="Z25" s="1"/>
+      <c r="Y25" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA25" s="49" t="s">
         <v>152</v>
       </c>
@@ -6153,7 +6271,7 @@
     </row>
     <row r="26" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
-        <f>COUNTIF(D26,"&lt;&gt;"&amp;"")+COUNTIF(BQ26,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B26" s="27">
@@ -6210,7 +6328,12 @@
       <c r="W26" t="s">
         <v>49</v>
       </c>
-      <c r="Z26" s="1"/>
+      <c r="Y26" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA26" s="49" t="s">
         <v>152</v>
       </c>
@@ -6300,7 +6423,7 @@
     </row>
     <row r="27" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A27" s="14">
-        <f>COUNTIF(D27,"&lt;&gt;"&amp;"")+COUNTIF(BQ27,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B27" s="27">
@@ -6357,7 +6480,12 @@
       <c r="W27" t="s">
         <v>49</v>
       </c>
-      <c r="Z27" s="1"/>
+      <c r="Y27" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA27" s="49" t="s">
         <v>152</v>
       </c>
@@ -6447,7 +6575,7 @@
     </row>
     <row r="28" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
-        <f>COUNTIF(D28,"&lt;&gt;"&amp;"")+COUNTIF(BQ28,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B28" s="27">
@@ -6504,7 +6632,12 @@
       <c r="W28" t="s">
         <v>49</v>
       </c>
-      <c r="Z28" s="1"/>
+      <c r="Y28" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA28" s="49" t="s">
         <v>152</v>
       </c>
@@ -6594,7 +6727,7 @@
     </row>
     <row r="29" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
-        <f>COUNTIF(D29,"&lt;&gt;"&amp;"")+COUNTIF(BQ29,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B29" s="27">
@@ -6651,7 +6784,12 @@
       <c r="W29" t="s">
         <v>49</v>
       </c>
-      <c r="Z29" s="1"/>
+      <c r="Y29" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA29" s="49" t="s">
         <v>152</v>
       </c>
@@ -6741,7 +6879,7 @@
     </row>
     <row r="30" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
-        <f>COUNTIF(D30,"&lt;&gt;"&amp;"")+COUNTIF(BQ30,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B30" s="27">
@@ -6798,7 +6936,12 @@
       <c r="W30" t="s">
         <v>49</v>
       </c>
-      <c r="Z30" s="1"/>
+      <c r="Y30" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA30" s="49" t="s">
         <v>152</v>
       </c>
@@ -6888,7 +7031,7 @@
     </row>
     <row r="31" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
-        <f>COUNTIF(D31,"&lt;&gt;"&amp;"")+COUNTIF(BQ31,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B31" s="27">
@@ -6945,7 +7088,12 @@
       <c r="W31" t="s">
         <v>49</v>
       </c>
-      <c r="Z31" s="1"/>
+      <c r="Y31" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA31" s="49" t="s">
         <v>152</v>
       </c>
@@ -7035,7 +7183,7 @@
     </row>
     <row r="32" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
-        <f>COUNTIF(D32,"&lt;&gt;"&amp;"")+COUNTIF(BQ32,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B32" s="27">
@@ -7092,7 +7240,12 @@
       <c r="W32" t="s">
         <v>49</v>
       </c>
-      <c r="Z32" s="1"/>
+      <c r="Y32" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA32" s="49" t="s">
         <v>152</v>
       </c>
@@ -7182,7 +7335,7 @@
     </row>
     <row r="33" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
-        <f>COUNTIF(D33,"&lt;&gt;"&amp;"")+COUNTIF(BQ33,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B33" s="27">
@@ -7239,7 +7392,12 @@
       <c r="W33" t="s">
         <v>49</v>
       </c>
-      <c r="Z33" s="1"/>
+      <c r="Y33" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA33" s="49" t="s">
         <v>152</v>
       </c>
@@ -7329,7 +7487,7 @@
     </row>
     <row r="34" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
-        <f>COUNTIF(D34,"&lt;&gt;"&amp;"")+COUNTIF(BQ34,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B34" s="27">
@@ -7386,7 +7544,12 @@
       <c r="W34" t="s">
         <v>49</v>
       </c>
-      <c r="Z34" s="1"/>
+      <c r="Y34" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA34" s="49" t="s">
         <v>152</v>
       </c>
@@ -7476,7 +7639,7 @@
     </row>
     <row r="35" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A35" s="14">
-        <f>COUNTIF(D35,"&lt;&gt;"&amp;"")+COUNTIF(BQ35,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B35" s="27">
@@ -7533,7 +7696,12 @@
       <c r="W35" t="s">
         <v>49</v>
       </c>
-      <c r="Z35" s="1"/>
+      <c r="Y35" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA35" s="49" t="s">
         <v>152</v>
       </c>
@@ -7623,7 +7791,7 @@
     </row>
     <row r="36" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A36" s="14">
-        <f>COUNTIF(D36,"&lt;&gt;"&amp;"")+COUNTIF(BQ36,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B36" s="27">
@@ -7680,7 +7848,12 @@
       <c r="W36" t="s">
         <v>49</v>
       </c>
-      <c r="Z36" s="1"/>
+      <c r="Y36" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z36" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA36" s="49" t="s">
         <v>152</v>
       </c>
@@ -7770,7 +7943,7 @@
     </row>
     <row r="37" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A37" s="14">
-        <f>COUNTIF(D37,"&lt;&gt;"&amp;"")+COUNTIF(BQ37,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B37" s="27">
@@ -7830,7 +8003,12 @@
         <v>49</v>
       </c>
       <c r="X37"/>
-      <c r="Y37"/>
+      <c r="Y37" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA37" s="49" t="s">
         <v>152</v>
       </c>
@@ -7920,7 +8098,7 @@
     </row>
     <row r="38" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A38" s="14">
-        <f>COUNTIF(D38,"&lt;&gt;"&amp;"")+COUNTIF(BQ38,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B38" s="27">
@@ -7980,7 +8158,12 @@
         <v>49</v>
       </c>
       <c r="X38"/>
-      <c r="Y38"/>
+      <c r="Y38" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AA38" s="49" t="s">
         <v>152</v>
       </c>
@@ -8227,19 +8410,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -8257,14 +8430,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>